<commit_message>
OB Table all countries (incl Shanghai)
</commit_message>
<xml_diff>
--- a/OB_Table_variable_overview_math_SUHAS.xlsx
+++ b/OB_Table_variable_overview_math_SUHAS.xlsx
@@ -13,16 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="Categories_for_latex (3)" sheetId="5" r:id="rId1"/>
-    <sheet name="Categories_for_latex (2)" sheetId="4" r:id="rId2"/>
-    <sheet name="Categories_for_latex" sheetId="3" r:id="rId3"/>
-    <sheet name="Categories" sheetId="2" r:id="rId4"/>
-    <sheet name="List" sheetId="1" r:id="rId5"/>
+    <sheet name="Indonesia Jordan" sheetId="6" r:id="rId2"/>
+    <sheet name="Categories_for_latex (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="Categories_for_latex" sheetId="3" r:id="rId4"/>
+    <sheet name="Categories" sheetId="2" r:id="rId5"/>
+    <sheet name="List" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Categories!$B$3:$S$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Categories_for_latex!$A$3:$T$55</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Categories_for_latex (2)'!$A$3:$T$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Categories!$B$3:$S$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Categories_for_latex!$A$3:$T$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Categories_for_latex (2)'!$A$3:$T$55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Categories_for_latex (3)'!$A$3:$T$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Indonesia Jordan'!$A$3:$H$55</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="72">
   <si>
     <t>Wealth</t>
   </si>
@@ -1157,8 +1159,8 @@
   </sheetPr>
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Y37" sqref="Y37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4902,11 +4904,1760 @@
     <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="64" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M67"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="9" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="105"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="107" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="107" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="107" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="61"/>
+      <c r="C6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109">
+        <v>197.30240000000001</v>
+      </c>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109">
+        <v>220.3262</v>
+      </c>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109">
+        <v>88.554699999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10">
+        <v>-1.3536999999999999</v>
+      </c>
+      <c r="E7" s="10">
+        <v>-17.271000000000001</v>
+      </c>
+      <c r="F7" s="10">
+        <v>6.1003999999999996</v>
+      </c>
+      <c r="G7" s="10">
+        <v>8.8937000000000008</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-0.84889999999999999</v>
+      </c>
+      <c r="I7" s="10">
+        <v>-3.5329000000000002</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2.4102999999999999</v>
+      </c>
+      <c r="E8" s="10">
+        <v>-6.5244999999999997</v>
+      </c>
+      <c r="F8" s="10">
+        <v>5.1805000000000003</v>
+      </c>
+      <c r="G8" s="10">
+        <v>-13.6441</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.3962</v>
+      </c>
+      <c r="I8" s="10">
+        <v>9.7698999999999998</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="110" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="10">
+        <v>-0.85450000000000004</v>
+      </c>
+      <c r="E9" s="10">
+        <v>18.0457</v>
+      </c>
+      <c r="F9" s="10">
+        <v>11.788500000000001</v>
+      </c>
+      <c r="G9" s="10">
+        <v>-24.2972</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1.6305000000000001</v>
+      </c>
+      <c r="I9" s="10">
+        <v>-17.898</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="10">
+        <v>-4.6096000000000004</v>
+      </c>
+      <c r="E10" s="10">
+        <v>-1.3158000000000001</v>
+      </c>
+      <c r="F10" s="10">
+        <v>6.8209999999999997</v>
+      </c>
+      <c r="G10" s="10">
+        <v>12.3146</v>
+      </c>
+      <c r="H10" s="10">
+        <v>-1.772</v>
+      </c>
+      <c r="I10" s="10">
+        <v>-12.5189</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10">
+        <v>6.7927999999999997</v>
+      </c>
+      <c r="E11" s="10">
+        <v>12.321199999999999</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1.5262</v>
+      </c>
+      <c r="G11" s="10">
+        <v>12.497299999999999</v>
+      </c>
+      <c r="H11" s="10">
+        <v>5.2760999999999996</v>
+      </c>
+      <c r="I11" s="10">
+        <v>12.9491</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="10">
+        <v>-1.4518</v>
+      </c>
+      <c r="E12" s="10">
+        <v>4.2812000000000001</v>
+      </c>
+      <c r="F12" s="10">
+        <v>6.05</v>
+      </c>
+      <c r="G12" s="10">
+        <v>-2.0318999999999998</v>
+      </c>
+      <c r="H12" s="10">
+        <v>4.4974999999999996</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1.3579000000000001</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="10">
+        <v>-0.38800000000000001</v>
+      </c>
+      <c r="E13" s="10">
+        <v>-2.3087</v>
+      </c>
+      <c r="F13" s="10">
+        <v>-4.5979000000000001</v>
+      </c>
+      <c r="G13" s="10">
+        <v>-4.6768999999999998</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.72802</v>
+      </c>
+      <c r="I13" s="10">
+        <v>9.9718999999999998</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2.7530000000000001</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.12809999999999999</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3.4577</v>
+      </c>
+      <c r="G14" s="10">
+        <v>-0.34300000000000003</v>
+      </c>
+      <c r="H14" s="10">
+        <v>2.2711000000000001</v>
+      </c>
+      <c r="I14" s="10">
+        <v>-1.1408</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="10">
+        <v>-0.47270000000000001</v>
+      </c>
+      <c r="E15" s="10">
+        <v>31.4282</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1.103</v>
+      </c>
+      <c r="G15" s="10">
+        <v>-1.8785000000000001</v>
+      </c>
+      <c r="H15" s="10">
+        <v>-0.66930000000000001</v>
+      </c>
+      <c r="I15" s="10">
+        <v>-51.1404</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.22889999999999999</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.59970000000000001</v>
+      </c>
+      <c r="F16" s="10">
+        <v>-2.9600000000000001E-2</v>
+      </c>
+      <c r="G16" s="10">
+        <v>-5.3118999999999996</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.25390000000000001</v>
+      </c>
+      <c r="I16" s="10">
+        <v>-0.82220000000000004</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="10">
+        <v>-0.30420000000000003</v>
+      </c>
+      <c r="E17" s="10">
+        <v>2.7972999999999999</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1.7685999999999999</v>
+      </c>
+      <c r="G17" s="10">
+        <v>-0.86129999999999995</v>
+      </c>
+      <c r="H17" s="10">
+        <v>-0.30009999999999998</v>
+      </c>
+      <c r="I17" s="10">
+        <v>-0.12839999999999999</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="10">
+        <v>-6.9776999999999996</v>
+      </c>
+      <c r="E18" s="10">
+        <v>-9.7581000000000007</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="G18" s="10">
+        <v>-16.981000000000002</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1.0350999999999999</v>
+      </c>
+      <c r="I18" s="10">
+        <v>-24.555099999999999</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="10">
+        <v>-4.1399999999999999E-2</v>
+      </c>
+      <c r="E19" s="10">
+        <v>35.159100000000002</v>
+      </c>
+      <c r="F19" s="10">
+        <v>-0.87470000000000003</v>
+      </c>
+      <c r="G19" s="10">
+        <v>8.2309000000000001</v>
+      </c>
+      <c r="H19" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I19" s="10">
+        <v>65.847700000000003</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="10">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="E20" s="10">
+        <v>3.2715000000000001</v>
+      </c>
+      <c r="F20" s="10">
+        <v>-1.3139000000000001</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="H20" s="10">
+        <v>-0.64980000000000004</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1.8805000000000001</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="10">
+        <v>-8.0399999999999999E-2</v>
+      </c>
+      <c r="E21" s="10">
+        <v>-3.4670999999999998</v>
+      </c>
+      <c r="F21" s="10">
+        <v>-1.645</v>
+      </c>
+      <c r="G21" s="10">
+        <v>-0.1837</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.18129999999999999</v>
+      </c>
+      <c r="I21" s="10">
+        <v>-16.271799999999999</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="10">
+        <v>-0.63270000000000004</v>
+      </c>
+      <c r="E22" s="10">
+        <v>-15.960699999999999</v>
+      </c>
+      <c r="F22" s="10">
+        <v>-1.3721000000000001</v>
+      </c>
+      <c r="G22" s="10">
+        <v>-0.81389999999999996</v>
+      </c>
+      <c r="H22" s="10">
+        <v>-0.45600000000000002</v>
+      </c>
+      <c r="I22" s="10">
+        <v>-38.098599999999998</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.49180000000000001</v>
+      </c>
+      <c r="E23" s="10">
+        <v>-0.31680000000000003</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1.4125000000000001</v>
+      </c>
+      <c r="G23" s="10">
+        <v>-13.0502</v>
+      </c>
+      <c r="H23" s="10">
+        <v>-0.65780000000000005</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="10">
+        <v>-0.29899999999999999</v>
+      </c>
+      <c r="E24" s="10">
+        <v>-31.421299999999999</v>
+      </c>
+      <c r="F24" s="10">
+        <v>-3.8008999999999999</v>
+      </c>
+      <c r="G24" s="10">
+        <v>-17.7227</v>
+      </c>
+      <c r="H24" s="10">
+        <v>-8.1668000000000003</v>
+      </c>
+      <c r="I24" s="10">
+        <v>-15.187200000000001</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.1084</v>
+      </c>
+      <c r="E25" s="10">
+        <v>-1.5941000000000001</v>
+      </c>
+      <c r="F25" s="10">
+        <v>7.2211999999999996</v>
+      </c>
+      <c r="G25" s="10">
+        <v>-0.7671</v>
+      </c>
+      <c r="H25" s="10">
+        <v>7.9348000000000001</v>
+      </c>
+      <c r="I25" s="10">
+        <v>-0.23960000000000001</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="112">
+        <f>SUM(D7:D25)</f>
+        <v>-4.5873000000000017</v>
+      </c>
+      <c r="E26" s="112">
+        <f>SUM(E7:E25)</f>
+        <v>18.093900000000005</v>
+      </c>
+      <c r="F26" s="112">
+        <f t="shared" ref="F26" si="0">SUM(F7:F25)</f>
+        <v>39.302700000000002</v>
+      </c>
+      <c r="G26" s="112">
+        <f>SUM(G7:G25)</f>
+        <v>-58.620900000000006</v>
+      </c>
+      <c r="H26" s="112">
+        <f>SUM(H7:H25)</f>
+        <v>10.68432</v>
+      </c>
+      <c r="I26" s="128">
+        <f>SUM(I7:I25)</f>
+        <v>-79.557899999999989</v>
+      </c>
+      <c r="J26" s="115"/>
+      <c r="K26" s="115"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="114">
+        <f>D26/$E$53</f>
+        <v>-6.2600301313333134E-2</v>
+      </c>
+      <c r="E27" s="114">
+        <f>E26/$E$53</f>
+        <v>0.24691726983919043</v>
+      </c>
+      <c r="F27" s="114">
+        <f>F26/$G$53</f>
+        <v>0.34919719925769149</v>
+      </c>
+      <c r="G27" s="114">
+        <f>G26/$G$53</f>
+        <v>-0.52083582293239927</v>
+      </c>
+      <c r="H27" s="114">
+        <f>H26/I53</f>
+        <v>-0.12394930759725942</v>
+      </c>
+      <c r="I27" s="114">
+        <f>I26/I53</f>
+        <v>0.92295500498787053</v>
+      </c>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="115">
+        <v>2.6597</v>
+      </c>
+      <c r="E28" s="115">
+        <v>-0.62239999999999995</v>
+      </c>
+      <c r="F28" s="115">
+        <v>-2.6800000000000001E-2</v>
+      </c>
+      <c r="G28" s="115">
+        <v>0.71220000000000006</v>
+      </c>
+      <c r="H28" s="115">
+        <v>1.5828</v>
+      </c>
+      <c r="I28" s="115">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="115">
+        <v>1.1331</v>
+      </c>
+      <c r="E29" s="115">
+        <v>-0.24399999999999999</v>
+      </c>
+      <c r="F29" s="115">
+        <v>3.0066000000000002</v>
+      </c>
+      <c r="G29" s="115">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="H29" s="115">
+        <v>1.0185999999999999</v>
+      </c>
+      <c r="I29" s="115">
+        <v>0.38890000000000002</v>
+      </c>
+      <c r="J29" s="115"/>
+      <c r="K29" s="115"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="115">
+        <v>-10.6968</v>
+      </c>
+      <c r="E30" s="115">
+        <v>-28.5366</v>
+      </c>
+      <c r="F30" s="115">
+        <v>23.194099999999999</v>
+      </c>
+      <c r="G30" s="115">
+        <v>-63.077399999999997</v>
+      </c>
+      <c r="H30" s="115">
+        <v>1.2012</v>
+      </c>
+      <c r="I30" s="115">
+        <v>-2.4455</v>
+      </c>
+      <c r="J30" s="115"/>
+      <c r="K30" s="115"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="115">
+        <v>0.42149999999999999</v>
+      </c>
+      <c r="E31" s="115">
+        <v>-18.447500000000002</v>
+      </c>
+      <c r="F31" s="115">
+        <v>-3.8340000000000001</v>
+      </c>
+      <c r="G31" s="115">
+        <v>24.301100000000002</v>
+      </c>
+      <c r="H31" s="115">
+        <v>-3.1122000000000001</v>
+      </c>
+      <c r="I31" s="115">
+        <v>-8.4981000000000009</v>
+      </c>
+      <c r="J31" s="115"/>
+      <c r="K31" s="115"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="115">
+        <v>-3.7307999999999999</v>
+      </c>
+      <c r="E32" s="115">
+        <v>3.9064999999999999</v>
+      </c>
+      <c r="F32" s="115">
+        <v>-4.5879000000000003</v>
+      </c>
+      <c r="G32" s="115">
+        <v>-17.802</v>
+      </c>
+      <c r="H32" s="115">
+        <v>-8.0828000000000007</v>
+      </c>
+      <c r="I32" s="115">
+        <v>-1.1654</v>
+      </c>
+      <c r="J32" s="115"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="113" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="115">
+        <v>-1.5344</v>
+      </c>
+      <c r="E33" s="115">
+        <v>-3.2852000000000001</v>
+      </c>
+      <c r="F33" s="115">
+        <v>-0.84379999999999999</v>
+      </c>
+      <c r="G33" s="115">
+        <v>9.0344999999999995</v>
+      </c>
+      <c r="H33" s="115">
+        <v>-3.3967000000000001</v>
+      </c>
+      <c r="I33" s="115">
+        <v>3.5560999999999998</v>
+      </c>
+      <c r="J33" s="115"/>
+      <c r="K33" s="115"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="115">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="E34" s="115">
+        <v>4.6253000000000002</v>
+      </c>
+      <c r="F34" s="115">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="G34" s="115">
+        <v>5.3532000000000002</v>
+      </c>
+      <c r="H34" s="115">
+        <v>2.4335</v>
+      </c>
+      <c r="I34" s="115">
+        <v>-2.6004</v>
+      </c>
+      <c r="J34" s="115"/>
+      <c r="K34" s="115"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="113" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="115">
+        <v>0.2273</v>
+      </c>
+      <c r="E35" s="115">
+        <v>-4.7899999999999998E-2</v>
+      </c>
+      <c r="F35" s="115">
+        <v>-0.50560000000000005</v>
+      </c>
+      <c r="G35" s="115">
+        <v>0.28239999999999998</v>
+      </c>
+      <c r="H35" s="115">
+        <v>0.92420000000000002</v>
+      </c>
+      <c r="I35" s="115">
+        <v>-2.4857</v>
+      </c>
+      <c r="J35" s="115"/>
+      <c r="K35" s="115"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="113" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="115">
+        <v>-6.2788000000000004</v>
+      </c>
+      <c r="E36" s="115">
+        <v>-2.0394000000000001</v>
+      </c>
+      <c r="F36" s="115">
+        <v>-2.8570000000000002</v>
+      </c>
+      <c r="G36" s="115">
+        <v>-5.5975999999999999</v>
+      </c>
+      <c r="H36" s="115">
+        <v>-9.2127999999999997</v>
+      </c>
+      <c r="I36" s="115">
+        <v>-0.1094</v>
+      </c>
+      <c r="J36" s="115"/>
+      <c r="K36" s="115"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="113" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="115">
+        <v>-0.3221</v>
+      </c>
+      <c r="E37" s="115">
+        <v>-4.9515000000000002</v>
+      </c>
+      <c r="F37" s="115">
+        <v>0.15970000000000001</v>
+      </c>
+      <c r="G37" s="115">
+        <v>0.85029999999999994</v>
+      </c>
+      <c r="H37" s="115">
+        <v>-0.77049999999999996</v>
+      </c>
+      <c r="I37" s="115">
+        <v>-8.6599000000000004</v>
+      </c>
+      <c r="J37" s="115"/>
+      <c r="K37" s="115"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="110" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="115">
+        <v>2.7490000000000001</v>
+      </c>
+      <c r="E38" s="115">
+        <v>-10.973699999999999</v>
+      </c>
+      <c r="F38" s="115">
+        <v>3.2614000000000001</v>
+      </c>
+      <c r="G38" s="115">
+        <v>-33.462699999999998</v>
+      </c>
+      <c r="H38" s="115">
+        <v>2.5554999999999999</v>
+      </c>
+      <c r="I38" s="115">
+        <v>-0.76200000000000001</v>
+      </c>
+      <c r="J38" s="115"/>
+      <c r="K38" s="115"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="110" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="115">
+        <v>-3.6669999999999998</v>
+      </c>
+      <c r="E39" s="115">
+        <v>-20.323899999999998</v>
+      </c>
+      <c r="F39" s="115">
+        <v>-8.5485000000000007</v>
+      </c>
+      <c r="G39" s="115">
+        <v>10.7592</v>
+      </c>
+      <c r="H39" s="115">
+        <v>-2.2002999999999999</v>
+      </c>
+      <c r="I39" s="115">
+        <v>-21.9057</v>
+      </c>
+      <c r="J39" s="115"/>
+      <c r="K39" s="115"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="110" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="115">
+        <v>4.7077999999999998</v>
+      </c>
+      <c r="E40" s="115">
+        <v>-9.8512000000000004</v>
+      </c>
+      <c r="F40" s="115">
+        <v>-2.34511</v>
+      </c>
+      <c r="G40" s="115">
+        <v>1.3381000000000001</v>
+      </c>
+      <c r="H40" s="115">
+        <v>1.2575000000000001</v>
+      </c>
+      <c r="I40" s="115">
+        <v>-2.1</v>
+      </c>
+      <c r="J40" s="115"/>
+      <c r="K40" s="115"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="110" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="115">
+        <v>-4.4467999999999996</v>
+      </c>
+      <c r="E41" s="115">
+        <v>1.0381</v>
+      </c>
+      <c r="F41" s="115">
+        <v>3.9636</v>
+      </c>
+      <c r="G41" s="115">
+        <v>1.4813000000000001</v>
+      </c>
+      <c r="H41" s="115">
+        <v>-3.4883999999999999</v>
+      </c>
+      <c r="I41" s="115">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="J41" s="115"/>
+      <c r="K41" s="115"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="110" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="115">
+        <v>27.683599999999998</v>
+      </c>
+      <c r="E42" s="115">
+        <v>-19.989100000000001</v>
+      </c>
+      <c r="F42" s="115">
+        <v>3.4112</v>
+      </c>
+      <c r="G42" s="115">
+        <v>7.9172000000000002</v>
+      </c>
+      <c r="H42" s="115">
+        <v>8.2979000000000003</v>
+      </c>
+      <c r="I42" s="115">
+        <v>4.5457999999999998</v>
+      </c>
+      <c r="J42" s="115"/>
+      <c r="K42" s="115"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="115">
+        <v>3.5728</v>
+      </c>
+      <c r="E43" s="115">
+        <v>-3.3755999999999999</v>
+      </c>
+      <c r="F43" s="115">
+        <v>6.7826000000000004</v>
+      </c>
+      <c r="G43" s="115">
+        <v>6.9161999999999999</v>
+      </c>
+      <c r="H43" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="I43" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="J43" s="115"/>
+      <c r="K43" s="115"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="115">
+        <v>-9.3596000000000004</v>
+      </c>
+      <c r="E44" s="115">
+        <v>-2.0706000000000002</v>
+      </c>
+      <c r="F44" s="115">
+        <v>-11.82</v>
+      </c>
+      <c r="G44" s="115">
+        <v>0.9214</v>
+      </c>
+      <c r="H44" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="J44" s="115"/>
+      <c r="K44" s="115"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="115">
+        <v>0.18770000000000001</v>
+      </c>
+      <c r="E45" s="115">
+        <v>1.3994</v>
+      </c>
+      <c r="F45" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" s="125">
+        <v>0.19617000000000001</v>
+      </c>
+      <c r="I45" s="125">
+        <v>-5.3329000000000004</v>
+      </c>
+      <c r="J45" s="115"/>
+      <c r="K45" s="115"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="115">
+        <v>0.26819999999999999</v>
+      </c>
+      <c r="E46" s="115">
+        <v>-8.9641000000000002</v>
+      </c>
+      <c r="F46" s="115">
+        <v>-0.35499999999999998</v>
+      </c>
+      <c r="G46" s="115">
+        <v>-19.7408</v>
+      </c>
+      <c r="H46" s="123">
+        <v>0.22919999999999999</v>
+      </c>
+      <c r="I46" s="123">
+        <v>-3.3761000000000001</v>
+      </c>
+      <c r="J46" s="115"/>
+      <c r="K46" s="115"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="115">
+        <v>7.5765000000000002</v>
+      </c>
+      <c r="E47" s="115">
+        <v>-21.464400000000001</v>
+      </c>
+      <c r="F47" s="115">
+        <v>1.8274999999999999</v>
+      </c>
+      <c r="G47" s="115">
+        <v>-7.3367000000000004</v>
+      </c>
+      <c r="H47" s="123">
+        <v>7.9599000000000002</v>
+      </c>
+      <c r="I47" s="123">
+        <v>-8.3436000000000003</v>
+      </c>
+      <c r="J47" s="115"/>
+      <c r="K47" s="115"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="115">
+        <v>-21.848400000000002</v>
+      </c>
+      <c r="E48" s="115">
+        <v>10.7935</v>
+      </c>
+      <c r="F48" s="115">
+        <v>-2.7900999999999998</v>
+      </c>
+      <c r="G48" s="115">
+        <v>-17.253799999999998</v>
+      </c>
+      <c r="H48" s="123">
+        <v>-11.366400000000001</v>
+      </c>
+      <c r="I48" s="123">
+        <v>-1.2101999999999999</v>
+      </c>
+      <c r="J48" s="115"/>
+      <c r="K48" s="115"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="115">
+        <v>0.69269999999999998</v>
+      </c>
+      <c r="E49" s="115">
+        <v>3.9018000000000002</v>
+      </c>
+      <c r="F49" s="115">
+        <v>0.154</v>
+      </c>
+      <c r="G49" s="115">
+        <v>-3.1366999999999998</v>
+      </c>
+      <c r="H49" s="123">
+        <v>0.72719999999999996</v>
+      </c>
+      <c r="I49" s="123">
+        <v>-32.196300000000001</v>
+      </c>
+      <c r="J49" s="115"/>
+      <c r="K49" s="115"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="112">
+        <f t="shared" ref="D50:E50" si="1">SUM(D28:D49)</f>
+        <v>-8.0073000000000008</v>
+      </c>
+      <c r="E50" s="112">
+        <f t="shared" si="1"/>
+        <v>-129.52250000000001</v>
+      </c>
+      <c r="F50" s="112">
+        <f>SUM(F28:F49)</f>
+        <v>8.1311900000000001</v>
+      </c>
+      <c r="G50" s="112">
+        <f>SUM(G28:G49)</f>
+        <v>-96.587599999999981</v>
+      </c>
+      <c r="H50" s="112">
+        <f>SUM(H28:H49)</f>
+        <v>-13.246429999999997</v>
+      </c>
+      <c r="I50" s="112">
+        <f>SUM(I28:I49)</f>
+        <v>-92.633800000000008</v>
+      </c>
+      <c r="J50" s="115"/>
+      <c r="K50" s="115"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="114">
+        <f>D50/$E$53</f>
+        <v>-0.10927111649690499</v>
+      </c>
+      <c r="E51" s="114">
+        <f>E50/$E$53</f>
+        <v>-1.7675206607059029</v>
+      </c>
+      <c r="F51" s="114">
+        <f>F50/$G$53</f>
+        <v>7.2244114898776635E-2</v>
+      </c>
+      <c r="G51" s="114">
+        <f>G50/$G$53</f>
+        <v>-0.85816291000420308</v>
+      </c>
+      <c r="H51" s="114">
+        <f>H50/I53</f>
+        <v>0.1536724683120278</v>
+      </c>
+      <c r="I51" s="114">
+        <f>I50/I53</f>
+        <v>1.0746491466095185</v>
+      </c>
+      <c r="J51" s="115"/>
+      <c r="K51" s="115"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="112">
+        <f t="shared" ref="D52" si="2">D26+D50</f>
+        <v>-12.594600000000003</v>
+      </c>
+      <c r="E52" s="112">
+        <f>E26+E50</f>
+        <v>-111.4286</v>
+      </c>
+      <c r="F52" s="112">
+        <f>F26+F50</f>
+        <v>47.433890000000005</v>
+      </c>
+      <c r="G52" s="112">
+        <f>G26+G50</f>
+        <v>-155.20849999999999</v>
+      </c>
+      <c r="H52" s="112">
+        <f>H26+H50</f>
+        <v>-2.562109999999997</v>
+      </c>
+      <c r="I52" s="128">
+        <f>I26+I50</f>
+        <v>-172.1917</v>
+      </c>
+      <c r="J52" s="115"/>
+      <c r="K52" s="115"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="126"/>
+      <c r="E53" s="127">
+        <f>D52+E52+E6</f>
+        <v>73.279200000000003</v>
+      </c>
+      <c r="F53" s="126"/>
+      <c r="G53" s="127">
+        <f>F52+G52+G6</f>
+        <v>112.55159000000002</v>
+      </c>
+      <c r="H53" s="127"/>
+      <c r="I53" s="127">
+        <f>H52+I52+I6</f>
+        <v>-86.19910999999999</v>
+      </c>
+      <c r="J53" s="115"/>
+      <c r="K53" s="115"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
+      <c r="F54" s="115"/>
+      <c r="G54" s="115"/>
+      <c r="H54" s="115"/>
+      <c r="I54" s="115"/>
+      <c r="J54" s="115"/>
+      <c r="K54" s="115"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="115"/>
+      <c r="F55" s="115"/>
+      <c r="G55" s="115"/>
+      <c r="H55" s="115"/>
+      <c r="I55" s="115"/>
+      <c r="J55" s="115"/>
+      <c r="K55" s="115"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="115"/>
+      <c r="E56" s="115"/>
+      <c r="F56" s="115"/>
+      <c r="G56" s="115"/>
+      <c r="H56" s="115"/>
+      <c r="I56" s="115"/>
+      <c r="J56" s="115"/>
+      <c r="K56" s="115"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="10"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="64" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8173,7 +9924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11441,7 +13192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -14244,7 +15995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E34"/>
   <sheetViews>

</xml_diff>